<commit_message>
Added Selenium Custom Driver
</commit_message>
<xml_diff>
--- a/CredenceWeb_DataSource/MasterData.xlsx
+++ b/CredenceWeb_DataSource/MasterData.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="Devices" sheetId="2" r:id="rId2"/>
+    <sheet name="Valid_LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="InValid_LoginCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>credencetestc5@gmail.com</t>
+  </si>
+  <si>
+    <t>vijeth35@gmail.com</t>
+  </si>
+  <si>
+    <t>TestDemo123</t>
   </si>
 </sst>
 </file>
@@ -128,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,6 +146,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,42 +480,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -514,30 +491,88 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A6" r:id="rId6"/>
-    <hyperlink ref="A7" r:id="rId7"/>
-    <hyperlink ref="B3:B7" r:id="rId8" display="India@12345"/>
-    <hyperlink ref="B3" r:id="rId9"/>
-    <hyperlink ref="B4" r:id="rId10"/>
-    <hyperlink ref="B5" r:id="rId11"/>
-    <hyperlink ref="B6" r:id="rId12"/>
-    <hyperlink ref="B7" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="B2:B6" r:id="rId6" display="India@12345"/>
+    <hyperlink ref="B2" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId9"/>
+    <hyperlink ref="B5" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId11"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>